<commit_message>
the student info is updated
</commit_message>
<xml_diff>
--- a/Student_info.xlsx
+++ b/Student_info.xlsx
@@ -11,15 +11,48 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Roll no</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Pass  or fail</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -42,12 +75,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,36 +461,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A3:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="E3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="5">
+        <v>101</v>
+      </c>
+      <c r="D4" s="9">
+        <v>86</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f>IF(D4&gt;35,"Pass","Fail")</f>
+        <v>Pass</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="5">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f t="shared" ref="E5:E14" si="0">IF(D5&gt;35,"Pass","Fail")</f>
+        <v>Pass</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="5">
+        <v>103</v>
+      </c>
+      <c r="D6" s="9">
+        <v>100</v>
+      </c>
+      <c r="E6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Pass</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="5">
+        <v>104</v>
+      </c>
+      <c r="D7" s="9">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Pass</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="5">
+        <v>105</v>
+      </c>
+      <c r="D8" s="9">
+        <v>31</v>
+      </c>
+      <c r="E8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Fail</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="5">
+        <v>106</v>
+      </c>
+      <c r="D9" s="9">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Fail</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="5">
+        <v>107</v>
+      </c>
+      <c r="D10" s="9">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Pass</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="5">
+        <v>108</v>
+      </c>
+      <c r="D11" s="9">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Pass</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="5">
+        <v>109</v>
+      </c>
+      <c r="D12" s="9">
+        <v>98</v>
+      </c>
+      <c r="E12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Pass</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="7">
+        <v>110</v>
+      </c>
+      <c r="D13" s="10">
+        <v>23</v>
+      </c>
+      <c r="E13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Fail</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
+      <c r="D14" s="4">
+        <f>SUM(D4:D13)</f>
+        <v>597</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Task given by principal:
</commit_message>
<xml_diff>
--- a/Student_info.xlsx
+++ b/Student_info.xlsx
@@ -13,6 +13,23 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t xml:space="preserve">roll </t>
+  </si>
+  <si>
+    <t>marks</t>
+  </si>
+  <si>
+    <t>pass or fail</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +59,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,33 +382,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="C3:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>